<commit_message>
feat(Examples): Add audio files of coral-reef-light campaign + Update xlsx and h5
</commit_message>
<xml_diff>
--- a/examples/campaigns/coral-reef-light/coral-reef.xlsx
+++ b/examples/campaigns/coral-reef-light/coral-reef.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="248">
   <si>
     <t xml:space="preserve">Sound Scape Explorer</t>
   </si>
@@ -565,7 +565,13 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/bamdad/git/sound-scape-explorer/sample-lana/audio</t>
+    <t xml:space="preserve">storage_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coral-reef.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio</t>
   </si>
   <si>
     <t xml:space="preserve">http://localhost:5531</t>
@@ -1471,7 +1477,7 @@
   </sheetPr>
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1892,22 +1898,22 @@
         <v>64</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B2" s="23" t="n">
         <v>15</v>
@@ -1924,7 +1930,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B3" s="30" t="n">
         <v>15</v>
@@ -1991,10 +1997,10 @@
         <v>49</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>56</v>
@@ -2002,7 +2008,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>44881.5</v>
@@ -2011,18 +2017,18 @@
         <v>44882.5034722222</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B3" s="27" t="n">
         <v>44887.5</v>
@@ -2031,18 +2037,18 @@
         <v>44888.5034722222</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B4" s="27" t="n">
         <v>44907.5</v>
@@ -2051,13 +2057,13 @@
         <v>44908.5034722222</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,82 +2115,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="34" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="34" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2223,74 +2229,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="36" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="34" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="34" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2336,12 +2342,12 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="34" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2380,17 +2386,17 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="34" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="34" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2433,22 +2439,22 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="34" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="34" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="34" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="34" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2468,9 +2474,9 @@
     <tabColor rgb="FFFFFFD7"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2495,69 +2501,77 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>83</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="15" t="n">
-        <v>44100</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="15" t="n">
+        <v>44100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="17" t="n">
+      <c r="B6" s="17" t="n">
         <v>44197</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="19" t="n">
-        <v>5</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="19" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="19" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="19" t="n">
+      <c r="B10" s="19" t="n">
         <v>42000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="http://localhost:5531"/>
+    <hyperlink ref="B4" r:id="rId1" display="http://localhost:5531"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2578,11 +2592,11 @@
   <dimension ref="A1:S55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2607,66 +2621,66 @@
         <v>26</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M1" s="25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="R1" s="25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="S1" s="25" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="27" t="n">
         <v>44881.5034722222</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2" s="23" t="n">
         <v>2022</v>
@@ -2681,22 +2695,22 @@
         <v>5</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O2" s="24" t="n">
         <v>465</v>
@@ -2711,21 +2725,21 @@
         <v>58</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C3" s="27" t="n">
         <v>44881.5104166667</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E3" s="23" t="n">
         <v>2022</v>
@@ -2740,22 +2754,22 @@
         <v>5</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O3" s="24" t="n">
         <v>465</v>
@@ -2770,21 +2784,21 @@
         <v>58</v>
       </c>
       <c r="S3" s="24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C4" s="27" t="n">
         <v>44881.5173611111</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="23" t="n">
         <v>2022</v>
@@ -2799,22 +2813,22 @@
         <v>5</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O4" s="24" t="n">
         <v>465</v>
@@ -2829,21 +2843,21 @@
         <v>58</v>
       </c>
       <c r="S4" s="24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C5" s="28" t="n">
         <v>44887.5</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E5" s="23" t="n">
         <v>2022</v>
@@ -2858,22 +2872,22 @@
         <v>5</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N5" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O5" s="24" t="n">
         <v>465</v>
@@ -2888,21 +2902,21 @@
         <v>58</v>
       </c>
       <c r="S5" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C6" s="28" t="n">
         <v>44887.5069444444</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E6" s="23" t="n">
         <v>2022</v>
@@ -2917,22 +2931,22 @@
         <v>5</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O6" s="24" t="n">
         <v>465</v>
@@ -2947,21 +2961,21 @@
         <v>58</v>
       </c>
       <c r="S6" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C7" s="28" t="n">
         <v>44887.5138888889</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E7" s="23" t="n">
         <v>2022</v>
@@ -2976,22 +2990,22 @@
         <v>5</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O7" s="24" t="n">
         <v>465</v>
@@ -3006,21 +3020,21 @@
         <v>58</v>
       </c>
       <c r="S7" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C8" s="28" t="n">
         <v>44907.5034722222</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E8" s="23" t="n">
         <v>2022</v>
@@ -3035,22 +3049,22 @@
         <v>5</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O8" s="24" t="n">
         <v>465</v>
@@ -3065,21 +3079,21 @@
         <v>58</v>
       </c>
       <c r="S8" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C9" s="28" t="n">
         <v>44907.5104166667</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E9" s="23" t="n">
         <v>2022</v>
@@ -3094,22 +3108,22 @@
         <v>5</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O9" s="24" t="n">
         <v>465</v>
@@ -3124,21 +3138,21 @@
         <v>58</v>
       </c>
       <c r="S9" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C10" s="28" t="n">
         <v>44907.5173611111</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E10" s="23" t="n">
         <v>2022</v>
@@ -3153,22 +3167,22 @@
         <v>5</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K10" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M10" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N10" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O10" s="24" t="n">
         <v>465</v>
@@ -3183,21 +3197,21 @@
         <v>58</v>
       </c>
       <c r="S10" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C11" s="28" t="n">
         <v>44881.5034722222</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E11" s="23" t="n">
         <v>2022</v>
@@ -3212,22 +3226,22 @@
         <v>2</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K11" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N11" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O11" s="24" t="n">
         <v>378</v>
@@ -3242,21 +3256,21 @@
         <v>44</v>
       </c>
       <c r="S11" s="24" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C12" s="28" t="n">
         <v>44881.5104166667</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E12" s="23" t="n">
         <v>2022</v>
@@ -3271,22 +3285,22 @@
         <v>2</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L12" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M12" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N12" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O12" s="24" t="n">
         <v>378</v>
@@ -3301,21 +3315,21 @@
         <v>44</v>
       </c>
       <c r="S12" s="24" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C13" s="28" t="n">
         <v>44881.5173611111</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E13" s="23" t="n">
         <v>2022</v>
@@ -3330,22 +3344,22 @@
         <v>2</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N13" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O13" s="24" t="n">
         <v>378</v>
@@ -3360,21 +3374,21 @@
         <v>44</v>
       </c>
       <c r="S13" s="24" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C14" s="28" t="n">
         <v>44887.5034722222</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E14" s="23" t="n">
         <v>2022</v>
@@ -3389,22 +3403,22 @@
         <v>2</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N14" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O14" s="24" t="n">
         <v>378</v>
@@ -3419,21 +3433,21 @@
         <v>44</v>
       </c>
       <c r="S14" s="24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C15" s="28" t="n">
         <v>44887.5104166667</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E15" s="23" t="n">
         <v>2022</v>
@@ -3448,22 +3462,22 @@
         <v>2</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L15" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N15" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O15" s="24" t="n">
         <v>378</v>
@@ -3478,21 +3492,21 @@
         <v>44</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C16" s="28" t="n">
         <v>44887.5173611111</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E16" s="23" t="n">
         <v>2022</v>
@@ -3507,22 +3521,22 @@
         <v>2</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M16" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N16" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O16" s="24" t="n">
         <v>378</v>
@@ -3537,21 +3551,21 @@
         <v>44</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C17" s="28" t="n">
         <v>44907.5</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E17" s="23" t="n">
         <v>2022</v>
@@ -3566,22 +3580,22 @@
         <v>2</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L17" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N17" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O17" s="24" t="n">
         <v>378</v>
@@ -3596,21 +3610,21 @@
         <v>44</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C18" s="28" t="n">
         <v>44907.5069444444</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E18" s="23" t="n">
         <v>2022</v>
@@ -3625,22 +3639,22 @@
         <v>2</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N18" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O18" s="24" t="n">
         <v>378</v>
@@ -3655,21 +3669,21 @@
         <v>44</v>
       </c>
       <c r="S18" s="24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C19" s="28" t="n">
         <v>44907.5138888889</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E19" s="23" t="n">
         <v>2022</v>
@@ -3684,22 +3698,22 @@
         <v>2</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L19" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N19" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O19" s="24" t="n">
         <v>378</v>
@@ -3714,21 +3728,21 @@
         <v>44</v>
       </c>
       <c r="S19" s="24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C20" s="28" t="n">
         <v>44881.5</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E20" s="23" t="n">
         <v>2022</v>
@@ -3743,22 +3757,22 @@
         <v>2</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L20" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N20" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O20" s="24" t="n">
         <v>509</v>
@@ -3773,21 +3787,21 @@
         <v>47</v>
       </c>
       <c r="S20" s="24" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C21" s="28" t="n">
         <v>44881.5069444444</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E21" s="23" t="n">
         <v>2022</v>
@@ -3802,22 +3816,22 @@
         <v>2</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L21" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N21" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O21" s="24" t="n">
         <v>509</v>
@@ -3832,21 +3846,21 @@
         <v>47</v>
       </c>
       <c r="S21" s="24" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C22" s="28" t="n">
         <v>44881.5138888889</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E22" s="23" t="n">
         <v>2022</v>
@@ -3861,22 +3875,22 @@
         <v>2</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K22" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M22" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N22" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O22" s="24" t="n">
         <v>509</v>
@@ -3891,21 +3905,21 @@
         <v>47</v>
       </c>
       <c r="S22" s="24" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="20" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C23" s="28" t="n">
         <v>44887.5034722222</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E23" s="23" t="n">
         <v>2022</v>
@@ -3920,22 +3934,22 @@
         <v>2</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N23" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O23" s="24" t="n">
         <v>509</v>
@@ -3950,21 +3964,21 @@
         <v>47</v>
       </c>
       <c r="S23" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C24" s="28" t="n">
         <v>44887.5104166667</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E24" s="23" t="n">
         <v>2022</v>
@@ -3979,22 +3993,22 @@
         <v>2</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O24" s="24" t="n">
         <v>509</v>
@@ -4009,21 +4023,21 @@
         <v>47</v>
       </c>
       <c r="S24" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C25" s="28" t="n">
         <v>44887.5173611111</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E25" s="23" t="n">
         <v>2022</v>
@@ -4038,22 +4052,22 @@
         <v>2</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L25" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N25" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O25" s="24" t="n">
         <v>509</v>
@@ -4068,21 +4082,21 @@
         <v>47</v>
       </c>
       <c r="S25" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C26" s="28" t="n">
         <v>44907.5034722222</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E26" s="23" t="n">
         <v>2022</v>
@@ -4097,22 +4111,22 @@
         <v>2</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O26" s="24" t="n">
         <v>509</v>
@@ -4127,21 +4141,21 @@
         <v>47</v>
       </c>
       <c r="S26" s="24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C27" s="28" t="n">
         <v>44907.5104166667</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E27" s="23" t="n">
         <v>2022</v>
@@ -4156,22 +4170,22 @@
         <v>2</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M27" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N27" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O27" s="24" t="n">
         <v>509</v>
@@ -4186,21 +4200,21 @@
         <v>47</v>
       </c>
       <c r="S27" s="24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C28" s="28" t="n">
         <v>44907.5173611111</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E28" s="23" t="n">
         <v>2022</v>
@@ -4215,22 +4229,22 @@
         <v>2</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N28" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O28" s="24" t="n">
         <v>509</v>
@@ -4245,21 +4259,21 @@
         <v>47</v>
       </c>
       <c r="S28" s="24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C29" s="28" t="n">
         <v>44243.5013888889</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E29" s="23" t="n">
         <v>2021</v>
@@ -4274,22 +4288,22 @@
         <v>2</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K29" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M29" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N29" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O29" s="24" t="n">
         <v>384</v>
@@ -4304,21 +4318,21 @@
         <v>60</v>
       </c>
       <c r="S29" s="24" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C30" s="28" t="n">
         <v>44243.5090277778</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E30" s="23" t="n">
         <v>2021</v>
@@ -4333,22 +4347,22 @@
         <v>2</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L30" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M30" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N30" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O30" s="24" t="n">
         <v>384</v>
@@ -4363,21 +4377,21 @@
         <v>60</v>
       </c>
       <c r="S30" s="24" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C31" s="28" t="n">
         <v>44243.5166666667</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E31" s="23" t="n">
         <v>2021</v>
@@ -4392,22 +4406,22 @@
         <v>2</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K31" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M31" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N31" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O31" s="24" t="n">
         <v>384</v>
@@ -4422,21 +4436,21 @@
         <v>60</v>
       </c>
       <c r="S31" s="24" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C32" s="28" t="n">
         <v>44273.5034722222</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E32" s="23" t="n">
         <v>2021</v>
@@ -4451,22 +4465,22 @@
         <v>2</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K32" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L32" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M32" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N32" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O32" s="24" t="n">
         <v>697</v>
@@ -4481,21 +4495,21 @@
         <v>72</v>
       </c>
       <c r="S32" s="24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C33" s="28" t="n">
         <v>44273.5111111111</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E33" s="23" t="n">
         <v>2021</v>
@@ -4510,22 +4524,22 @@
         <v>2</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K33" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L33" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M33" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N33" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O33" s="24" t="n">
         <v>697</v>
@@ -4540,21 +4554,21 @@
         <v>72</v>
       </c>
       <c r="S33" s="24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C34" s="28" t="n">
         <v>44273.51875</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E34" s="23" t="n">
         <v>2021</v>
@@ -4569,22 +4583,22 @@
         <v>2</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K34" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L34" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M34" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N34" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O34" s="24" t="n">
         <v>697</v>
@@ -4599,21 +4613,21 @@
         <v>72</v>
       </c>
       <c r="S34" s="24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C35" s="28" t="n">
         <v>44300.5034722222</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E35" s="23" t="n">
         <v>2021</v>
@@ -4628,22 +4642,22 @@
         <v>2</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K35" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L35" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M35" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N35" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O35" s="24" t="n">
         <v>1794</v>
@@ -4658,21 +4672,21 @@
         <v>146</v>
       </c>
       <c r="S35" s="24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C36" s="28" t="n">
         <v>44300.5111111111</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E36" s="23" t="n">
         <v>2021</v>
@@ -4687,22 +4701,22 @@
         <v>2</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K36" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L36" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M36" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N36" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O36" s="24" t="n">
         <v>1794</v>
@@ -4717,21 +4731,21 @@
         <v>146</v>
       </c>
       <c r="S36" s="24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C37" s="28" t="n">
         <v>44300.51875</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E37" s="23" t="n">
         <v>2021</v>
@@ -4746,22 +4760,22 @@
         <v>2</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K37" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L37" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M37" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N37" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O37" s="24" t="n">
         <v>1794</v>
@@ -4776,21 +4790,21 @@
         <v>146</v>
       </c>
       <c r="S37" s="24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C38" s="28" t="n">
         <v>44245.5041666667</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E38" s="23" t="n">
         <v>2021</v>
@@ -4805,22 +4819,22 @@
         <v>5</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K38" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L38" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M38" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N38" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O38" s="24" t="n">
         <v>352</v>
@@ -4835,21 +4849,21 @@
         <v>46</v>
       </c>
       <c r="S38" s="24" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="20" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C39" s="28" t="n">
         <v>44245.5118055556</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E39" s="23" t="n">
         <v>2021</v>
@@ -4864,22 +4878,22 @@
         <v>5</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K39" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L39" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M39" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N39" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O39" s="24" t="n">
         <v>352</v>
@@ -4894,21 +4908,21 @@
         <v>46</v>
       </c>
       <c r="S39" s="24" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C40" s="28" t="n">
         <v>44245.5194444444</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E40" s="23" t="n">
         <v>2021</v>
@@ -4923,22 +4937,22 @@
         <v>5</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L40" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M40" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N40" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O40" s="24" t="n">
         <v>352</v>
@@ -4953,21 +4967,21 @@
         <v>46</v>
       </c>
       <c r="S40" s="24" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="20" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C41" s="28" t="n">
         <v>44271.5027777778</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E41" s="23" t="n">
         <v>2021</v>
@@ -4982,22 +4996,22 @@
         <v>5</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K41" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L41" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M41" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N41" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O41" s="24" t="n">
         <v>497</v>
@@ -5012,21 +5026,21 @@
         <v>42</v>
       </c>
       <c r="S41" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C42" s="28" t="n">
         <v>44271.5104166667</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E42" s="23" t="n">
         <v>2021</v>
@@ -5041,22 +5055,22 @@
         <v>5</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K42" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L42" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M42" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N42" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O42" s="24" t="n">
         <v>497</v>
@@ -5071,21 +5085,21 @@
         <v>42</v>
       </c>
       <c r="S42" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="20" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C43" s="28" t="n">
         <v>44271.5180555556</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E43" s="23" t="n">
         <v>2021</v>
@@ -5100,22 +5114,22 @@
         <v>5</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K43" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L43" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M43" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N43" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O43" s="24" t="n">
         <v>497</v>
@@ -5130,21 +5144,21 @@
         <v>42</v>
       </c>
       <c r="S43" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C44" s="28" t="n">
         <v>44305.5027777778</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E44" s="23" t="n">
         <v>2021</v>
@@ -5159,22 +5173,22 @@
         <v>5</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J44" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K44" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L44" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M44" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N44" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O44" s="24" t="n">
         <v>1178</v>
@@ -5189,21 +5203,21 @@
         <v>90</v>
       </c>
       <c r="S44" s="24" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="20" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C45" s="28" t="n">
         <v>44305.5104166667</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E45" s="23" t="n">
         <v>2021</v>
@@ -5218,22 +5232,22 @@
         <v>5</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J45" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K45" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L45" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="M45" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N45" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O45" s="24" t="n">
         <v>1178</v>
@@ -5248,21 +5262,21 @@
         <v>90</v>
       </c>
       <c r="S45" s="24" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="20" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C46" s="28" t="n">
         <v>44305.5180555556</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E46" s="23" t="n">
         <v>2021</v>
@@ -5277,22 +5291,22 @@
         <v>5</v>
       </c>
       <c r="I46" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K46" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L46" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M46" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N46" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O46" s="24" t="n">
         <v>1178</v>
@@ -5307,21 +5321,21 @@
         <v>90</v>
       </c>
       <c r="S46" s="24" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="20" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C47" s="28" t="n">
         <v>44243.5055555556</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E47" s="23" t="n">
         <v>2021</v>
@@ -5336,22 +5350,22 @@
         <v>2</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K47" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L47" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M47" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N47" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O47" s="24" t="n">
         <v>387</v>
@@ -5366,21 +5380,21 @@
         <v>54</v>
       </c>
       <c r="S47" s="24" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C48" s="28" t="n">
         <v>44243.5131944445</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E48" s="23" t="n">
         <v>2021</v>
@@ -5395,22 +5409,22 @@
         <v>2</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K48" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L48" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M48" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N48" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O48" s="24" t="n">
         <v>387</v>
@@ -5425,21 +5439,21 @@
         <v>54</v>
       </c>
       <c r="S48" s="24" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C49" s="28" t="n">
         <v>44243.5208333333</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E49" s="23" t="n">
         <v>2021</v>
@@ -5454,22 +5468,22 @@
         <v>2</v>
       </c>
       <c r="I49" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K49" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L49" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M49" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N49" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O49" s="24" t="n">
         <v>387</v>
@@ -5484,21 +5498,21 @@
         <v>54</v>
       </c>
       <c r="S49" s="24" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C50" s="28" t="n">
         <v>44273.5</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E50" s="23" t="n">
         <v>2021</v>
@@ -5513,22 +5527,22 @@
         <v>2</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K50" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L50" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M50" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N50" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O50" s="24" t="n">
         <v>680</v>
@@ -5543,21 +5557,21 @@
         <v>63</v>
       </c>
       <c r="S50" s="24" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C51" s="28" t="n">
         <v>44273.5076388889</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E51" s="23" t="n">
         <v>2021</v>
@@ -5572,22 +5586,22 @@
         <v>2</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J51" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K51" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L51" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M51" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N51" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O51" s="24" t="n">
         <v>680</v>
@@ -5602,21 +5616,21 @@
         <v>63</v>
       </c>
       <c r="S51" s="24" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C52" s="28" t="n">
         <v>44273.5152777778</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E52" s="23" t="n">
         <v>2021</v>
@@ -5631,22 +5645,22 @@
         <v>2</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K52" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L52" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M52" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N52" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O52" s="24" t="n">
         <v>680</v>
@@ -5661,21 +5675,21 @@
         <v>63</v>
       </c>
       <c r="S52" s="24" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C53" s="28" t="n">
         <v>44299.5069444445</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E53" s="23" t="n">
         <v>2021</v>
@@ -5690,22 +5704,22 @@
         <v>2</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K53" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L53" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M53" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N53" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O53" s="24" t="n">
         <v>1258</v>
@@ -5720,21 +5734,21 @@
         <v>86</v>
       </c>
       <c r="S53" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C54" s="28" t="n">
         <v>44299.5145833333</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E54" s="23" t="n">
         <v>2021</v>
@@ -5749,22 +5763,22 @@
         <v>2</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K54" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L54" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M54" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N54" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O54" s="24" t="n">
         <v>1258</v>
@@ -5779,21 +5793,21 @@
         <v>86</v>
       </c>
       <c r="S54" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C55" s="28" t="n">
         <v>44299.5222222222</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E55" s="23" t="n">
         <v>2021</v>
@@ -5808,22 +5822,22 @@
         <v>2</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K55" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="L55" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M55" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N55" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O55" s="24" t="n">
         <v>1258</v>
@@ -5838,7 +5852,7 @@
         <v>86</v>
       </c>
       <c r="S55" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -5888,7 +5902,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>70</v>
@@ -5953,7 +5967,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>15</v>
@@ -6015,7 +6029,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B2" s="27" t="n">
         <v>44562.5</v>
@@ -6026,7 +6040,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B3" s="27" t="n">
         <v>44881.5</v>
@@ -6037,7 +6051,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B4" s="28" t="n">
         <v>44887.5</v>
@@ -6048,7 +6062,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B5" s="28" t="n">
         <v>44907.5</v>
@@ -6106,7 +6120,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="30" t="n">
         <v>0</v>
@@ -6115,12 +6129,12 @@
         <v>1000</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B3" s="30" t="n">
         <v>0</v>
@@ -6129,12 +6143,12 @@
         <v>1000</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B4" s="30" t="n">
         <v>0</v>
@@ -6143,7 +6157,7 @@
         <v>1000</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -6189,17 +6203,17 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -6265,7 +6279,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B2" s="23" t="n">
         <v>2</v>
@@ -6276,7 +6290,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B3" s="30" t="n">
         <v>3</v>

</xml_diff>